<commit_message>
Minor formatting changes: 1. No index for output df; 2. Line indentation in zillowbot.py
</commit_message>
<xml_diff>
--- a/listings.xlsx
+++ b/listings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>Address</t>
   </si>
@@ -25,126 +25,135 @@
     <t>URL</t>
   </si>
   <si>
+    <t>1085 103rd Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Park 433 | 433 Bellevue Way SE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>537 Bellevue Way SE #1697806, Bellevue, WA 98004</t>
+  </si>
+  <si>
+    <t>Alley 111 | 11011 NE 9th St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>177 107th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Aventine | 211 112th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>12 Central Square | 10290 NE 12th St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Cerasa | 10961 NE 2nd Pl, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>City Square Bellevue | 938 110th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>10245 Main St #73JGW1E7W, Bellevue, WA 98004</t>
+  </si>
+  <si>
+    <t>Sylva on Main Apartments | 10701 Main St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Soma Towers | 288 106th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>88 102nd Ave NE #161KHGUNZ, Bellevue, WA 98004</t>
+  </si>
+  <si>
+    <t>Avalon Towers Bellevue | 10349 NE 10th St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Avalon Bellevue | 11000 NE 10th St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>AMLI Bellevue Park | 10001 NE 1st St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Metro 112 Apartments | 317 112th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Main Street Flats | 10575 Main St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>The Bravern | 688 110th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Borgata | 37 103rd Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Ashton Bellevue | 10710 NE 10th St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Two Lincoln Tower | 10485 NE 6th St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>1515 Bellevue Way NE #3375777, Bellevue, WA 98004</t>
+  </si>
+  <si>
+    <t>Venn at Main | 10333 NE 1st St, Bellevue, WA</t>
+  </si>
+  <si>
     <t>The Meyden | 10333 Main St, Bellevue, WA</t>
   </si>
   <si>
+    <t>Avalon Meydenbauer | 10410 NE 2nd St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Lux | 1000 100th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Brio | 11130 NE 10th St, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>BLU | 75 102nd Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Elements Apartments | 958 111th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>TEN20 | 1020 108th Ave NE, Bellevue, WA</t>
+  </si>
+  <si>
+    <t>11101 NE 12th St APT 107, Bellevue, WA 98004</t>
+  </si>
+  <si>
     <t>900 108th Ave NE | 900 108th Ave NE, Bellevue, WA</t>
   </si>
   <si>
     <t>300 110th Ave NE, Bellevue, WA</t>
   </si>
   <si>
-    <t>Park 433 | 433 Bellevue Way SE, Bellevue, WA</t>
+    <t>10305 NE 16th St APT I7, Bellevue, WA 98004</t>
   </si>
   <si>
     <t>410 102nd Ave SE, Bellevue, WA 98004</t>
   </si>
   <si>
-    <t>537 Bellevue Way SE #1697806, Bellevue, WA 98004</t>
-  </si>
-  <si>
-    <t>Alley 111 | 11011 NE 9th St, Bellevue, WA</t>
-  </si>
-  <si>
     <t>118 107th Ave NE #315, Bellevue, WA 98004</t>
   </si>
   <si>
-    <t>Aventine | 211 112th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Cerasa | 10961 NE 2nd Pl, Bellevue, WA</t>
-  </si>
-  <si>
     <t>9922 Lake Washington Blvd NE, Bellevue, WA</t>
   </si>
   <si>
-    <t>12 Central Square | 10290 NE 12th St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>10245 Main St #73JGW1E7W, Bellevue, WA 98004</t>
-  </si>
-  <si>
-    <t>Sylva on Main Apartments | 10701 Main St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Elements Apartments | 958 111th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>City Square Bellevue | 938 110th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Park 88 | 88 102nd Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Soma Towers | 288 106th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
     <t>650 Bellevue Way NE, Bellevue, WA</t>
   </si>
   <si>
-    <t>Avalon Towers Bellevue | 10349 NE 10th St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Avalon Bellevue | 11000 NE 10th St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>AMLI Bellevue Park | 10001 NE 1st St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Metro 112 Apartments | 317 112th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Main Street Flats | 10575 Main St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>The Bravern | 688 110th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>1515 Bellevue Way NE #1517H, Bellevue, WA 98004</t>
-  </si>
-  <si>
-    <t>Ashton Bellevue | 10710 NE 10th St, Bellevue, WA</t>
-  </si>
-  <si>
     <t>10610 NE 9th Pl, Bellevue, WA</t>
   </si>
   <si>
-    <t>Two Lincoln Tower | 10485 NE 6th St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Venn at Main | 10333 NE 1st St, Bellevue, WA</t>
+    <t>205 105th Ave SE, Bellevue, WA</t>
   </si>
   <si>
     <t>10650 NE 9th Pl UNIT 1524, Bellevue, WA 98004</t>
   </si>
   <si>
-    <t>Avalon Meydenbauer | 10410 NE 2nd St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>1085 103rd Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
     <t>1100 106th Ave NE APT 606, Bellevue, WA 98004</t>
   </si>
   <si>
-    <t>TEN20 | 1020 108th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Brio | 11130 NE 10th St, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>BLU | 75 102nd Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Borgata | 37 103rd Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Lux | 1000 100th Ave NE, Bellevue, WA</t>
-  </si>
-  <si>
-    <t>Park Metro | 11101 NE 12th St, Bellevue, WA</t>
-  </si>
-  <si>
     <t>1620 103rd Ave NE, Bellevue, WA 98004</t>
   </si>
   <si>
@@ -160,13 +169,7 @@
     <t>812 100th Ave NE, Bellevue, WA</t>
   </si>
   <si>
-    <t>102nd Ave NE #411, Bellevue, WA 98004</t>
-  </si>
-  <si>
-    <t>788 110th Ave NE, Bellevue, WA 98004</t>
-  </si>
-  <si>
-    <t>10700 NE 4th St, Bellevue, WA</t>
+    <t>10700 NE 4th St UNIT 428, Bellevue, WA 98004</t>
   </si>
   <si>
     <t>10008 NE 16th Pl #ADU, Bellevue, WA 98004</t>
@@ -190,9 +193,6 @@
     <t>10201 SE 3rd St #1, Bellevue, WA 98004</t>
   </si>
   <si>
-    <t>205 105th Ave SE, Bellevue, WA</t>
-  </si>
-  <si>
     <t>425 Bellevue Way SE #25, Bellevue, WA 98004</t>
   </si>
   <si>
@@ -211,129 +211,135 @@
     <t>125 108th Ave SE APT 12, Bellevue, WA 98004</t>
   </si>
   <si>
-    <t>177 107th Ave NE APT 708, Bellevue, WA 98004</t>
+    <t>https://www.zillow.com/b/1085-103rd-ave-ne-bellevue-wa-BG9pnD/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/park-433-bellevue-wa-9VSJsn/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/537-Bellevue-Way-SE-1697806-Bellevue-WA-98004/2098531044_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/alley-111-bellevue-wa-5zpjzy/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/177-107th-ave-ne-bellevue-wa-5Xrs4s/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/aventine-bellevue-wa-5XjKwL/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/12-central-square-bellevue-wa-5XjFqC/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/cerasa-bellevue-wa-BKR5YY/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/city-square-bellevue-bellevue-wa-5XkJ93/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/10245-Main-St-73JGW1E7W-Bellevue-WA-98004/2073066244_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/sylva-on-main-apartments-bellevue-wa-5Xnhwr/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/soma-towers-bellevue-wa-5bR2bQ/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/88-102nd-Ave-NE-161KHGUNZ-Bellevue-WA-98004/2070452484_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/avalon-towers-bellevue-bellevue-wa-5XjFg5/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/avalon-bellevue-bellevue-wa-5XjPfD/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/amli-bellevue-park-bellevue-wa-5Xj9VV/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/metro-112-apartments-bellevue-wa-5Xk5rF/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/main-street-flats-bellevue-wa-65ZSwC/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/the-bravern-bellevue-wa-5XjRT2/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/borgata-bellevue-wa-5XjRc4/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/ashton-bellevue-bellevue-wa-5XjV9N/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/two-lincoln-tower-bellevue-wa-BHmS47/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1515-Bellevue-Way-NE-3375777-Bellevue-WA-98004/2079933369_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/venn-at-main-bellevue-wa-9kBw6T/</t>
   </si>
   <si>
     <t>https://www.zillow.com/b/the-meyden-bellevue-wa-5hJ4p9/</t>
   </si>
   <si>
+    <t>https://www.zillow.com/b/avalon-meydenbauer-bellevue-wa-5XjGYw/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/lux-bellevue-wa-5Znksy/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/brio-bellevue-wa-BW9wC7/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/blu-bellevue-wa-BcxTVp/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/elements-apartments-bellevue-wa-5XjW4s/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/b/ten20-bellevue-wa-5XjQBF/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/11101-NE-12th-St-APT-107-Bellevue-WA-98004/2082985886_zpid/</t>
+  </si>
+  <si>
     <t>https://www.zillow.com/b/900-108th-ave-ne-bellevue-wa-5YJVG4/</t>
   </si>
   <si>
     <t>https://www.zillow.com/b/300-110th-ave-ne-bellevue-wa-5XkXpv/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/park-433-bellevue-wa-9VSJsn/</t>
+    <t>https://www.zillow.com/homedetails/10305-NE-16th-St-APT-I7-Bellevue-WA-98004/2070238834_zpid/</t>
   </si>
   <si>
     <t>https://www.zillow.com/homedetails/410-102nd-Ave-SE-Bellevue-WA-98004/2075772896_zpid/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/homedetails/537-Bellevue-Way-SE-1697806-Bellevue-WA-98004/2098531044_zpid/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/alley-111-bellevue-wa-5zpjzy/</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/118-107th-Ave-NE-315-Bellevue-WA-98004/2070243355_zpid/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/aventine-bellevue-wa-5XjKwL/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/cerasa-bellevue-wa-BKR5YY/</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/b/9922-lake-washington-blvd-ne-bellevue-wa-9VSKqF/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/12-central-square-bellevue-wa-5XjFqC/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/10245-Main-St-73JGW1E7W-Bellevue-WA-98004/2073066244_zpid/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/sylva-on-main-apartments-bellevue-wa-5Xnhwr/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/elements-apartments-bellevue-wa-5Xrfhq/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/city-square-bellevue-bellevue-wa-5XkJ93/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/park-88-bellevue-wa-65dNtS/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/soma-towers-bellevue-wa-5bR2bQ/</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/b/650-bellevue-way-ne-bellevue-wa-5XkDKg/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/avalon-towers-bellevue-bellevue-wa-5XjFg5/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/avalon-bellevue-bellevue-wa-5XjPfD/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/amli-bellevue-park-bellevue-wa-5Xj9VV/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/metro-112-apartments-bellevue-wa-5Xk5rF/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/main-street-flats-bellevue-wa-65ZSwC/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/the-bravern-bellevue-wa-5XjRT2/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1515-Bellevue-Way-NE-1517H-Bellevue-WA-98004/2080303325_zpid/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/ashton-bellevue-bellevue-wa-5XjV9N/</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/b/washington-square-towers-bellevue-wa-5XkKmT/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/two-lincoln-tower-bellevue-wa-BHmS47/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/venn-at-main-bellevue-wa-9kBw6T/</t>
+    <t>https://www.zillow.com/b/205-105th-ave-se-bellevue-wa-BzDfJd/</t>
   </si>
   <si>
     <t>https://www.zillow.com/homedetails/10650-NE-9th-Pl-UNIT-1524-Bellevue-WA-98004/2087878514_zpid/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/avalon-meydenbauer-bellevue-wa-5XjGYw/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/1085-103rd-ave-ne-bellevue-wa-BG9pnD/</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/1100-106th-Ave-NE-APT-606-Bellevue-WA-98004/58387391_zpid/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/ten20-bellevue-wa-5XjQBF/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/brio-bellevue-wa-BW9wC7/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/blu-bellevue-wa-BcxTVp/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/borgata-bellevue-wa-5XjRc4/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/lux-bellevue-wa-5Znksy/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/park-metro-bellevue-wa-5Yv2DD/</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/1620-103rd-Ave-NE-Bellevue-WA-98004/2104652731_zpid/</t>
   </si>
   <si>
@@ -349,13 +355,7 @@
     <t>https://www.zillow.com/b/812-100th-ave-ne-bellevue-wa-5jDpzz/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/homedetails/102nd-Ave-NE-411-Bellevue-WA-98004/2070419384_zpid/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/788-110th-Ave-NE-Bellevue-WA-98004/2070438155_zpid/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/b/10700-ne-4th-st-bellevue-wa-5XkPcQ/</t>
+    <t>https://www.zillow.com/homedetails/10700-NE-4th-St-UNIT-428-Bellevue-WA-98004/89210707_zpid/</t>
   </si>
   <si>
     <t>https://www.zillow.com/homedetails/10008-NE-16th-Pl-ADU-Bellevue-WA-98004/2072319855_zpid/</t>
@@ -379,9 +379,6 @@
     <t>https://www.zillow.com/homedetails/10201-SE-3rd-St-1-Bellevue-WA-98004/2070980862_zpid/</t>
   </si>
   <si>
-    <t>https://www.zillow.com/b/205-105th-ave-se-bellevue-wa-BzDfJd/</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/425-Bellevue-Way-SE-25-Bellevue-WA-98004/2071064509_zpid/</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
   </si>
   <si>
     <t>https://www.zillow.com/homedetails/125-108th-Ave-SE-APT-12-Bellevue-WA-98004/2111358457_zpid/</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/177-107th-Ave-NE-APT-708-Bellevue-WA-98004/48683313_zpid/</t>
   </si>
 </sst>
 </file>
@@ -771,7 +765,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -796,10 +790,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1788</v>
+        <v>1795</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -810,10 +804,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>1980</v>
+        <v>1795</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -824,10 +818,10 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2200</v>
+        <v>1650</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -838,10 +832,10 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>1795</v>
+        <v>1888</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -852,10 +846,10 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>2100</v>
+        <v>2450</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -866,10 +860,10 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1650</v>
+        <v>1736</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -880,10 +874,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>1888</v>
+        <v>2671</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -894,10 +888,10 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>2795</v>
+        <v>1970</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -908,10 +902,10 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>1736</v>
+        <v>1670</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -922,10 +916,10 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1785</v>
+        <v>2000</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -936,10 +930,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1550</v>
+        <v>1627</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -950,10 +944,10 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>2639</v>
+        <v>1915</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -964,10 +958,10 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2000</v>
+        <v>2250</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -978,10 +972,10 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>1627</v>
+        <v>1940</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -992,10 +986,10 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>1761</v>
+        <v>1790</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1006,10 +1000,10 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>1770</v>
+        <v>2035</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1020,10 +1014,10 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>2195</v>
+        <v>1875</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1034,10 +1028,10 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>1995</v>
+        <v>1710</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1048,10 +1042,10 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>4800</v>
+        <v>2165</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1062,10 +1056,10 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>1940</v>
+        <v>1855</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1076,10 +1070,10 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>1805</v>
+        <v>3299</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1090,10 +1084,10 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>2035</v>
+        <v>3902</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1104,10 +1098,10 @@
         <v>25</v>
       </c>
       <c r="C24">
-        <v>1885</v>
+        <v>2455</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1118,10 +1112,10 @@
         <v>26</v>
       </c>
       <c r="C25">
-        <v>1710</v>
+        <v>2355</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1132,10 +1126,10 @@
         <v>27</v>
       </c>
       <c r="C26">
-        <v>2315</v>
+        <v>1788</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1146,10 +1140,10 @@
         <v>28</v>
       </c>
       <c r="C27">
-        <v>2455</v>
+        <v>1765</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1160,10 +1154,10 @@
         <v>29</v>
       </c>
       <c r="C28">
-        <v>3299</v>
+        <v>2850</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1174,10 +1168,10 @@
         <v>30</v>
       </c>
       <c r="C29">
-        <v>2395</v>
+        <v>2265</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1188,10 +1182,10 @@
         <v>31</v>
       </c>
       <c r="C30">
-        <v>3902</v>
+        <v>2595</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1202,10 +1196,10 @@
         <v>32</v>
       </c>
       <c r="C31">
-        <v>2355</v>
+        <v>1761</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1216,10 +1210,10 @@
         <v>33</v>
       </c>
       <c r="C32">
-        <v>3800</v>
+        <v>3105</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1230,10 +1224,10 @@
         <v>34</v>
       </c>
       <c r="C33">
-        <v>1822</v>
+        <v>1780</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1244,10 +1238,10 @@
         <v>35</v>
       </c>
       <c r="C34">
-        <v>1795</v>
+        <v>1980</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1258,10 +1252,10 @@
         <v>36</v>
       </c>
       <c r="C35">
-        <v>1800</v>
+        <v>2200</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1272,10 +1266,10 @@
         <v>37</v>
       </c>
       <c r="C36">
-        <v>2949</v>
+        <v>3000</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1286,10 +1280,10 @@
         <v>38</v>
       </c>
       <c r="C37">
-        <v>2265</v>
+        <v>2100</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1300,10 +1294,10 @@
         <v>39</v>
       </c>
       <c r="C38">
-        <v>2245</v>
+        <v>2795</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1314,10 +1308,10 @@
         <v>40</v>
       </c>
       <c r="C39">
-        <v>1855</v>
+        <v>1550</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1328,10 +1322,10 @@
         <v>41</v>
       </c>
       <c r="C40">
-        <v>3075</v>
+        <v>4800</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1342,10 +1336,10 @@
         <v>42</v>
       </c>
       <c r="C41">
-        <v>1780</v>
+        <v>2700</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1356,10 +1350,10 @@
         <v>43</v>
       </c>
       <c r="C42">
-        <v>2649</v>
+        <v>2220</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1370,10 +1364,10 @@
         <v>44</v>
       </c>
       <c r="C43">
-        <v>4500</v>
+        <v>3800</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1384,10 +1378,10 @@
         <v>45</v>
       </c>
       <c r="C44">
-        <v>1900</v>
+        <v>1800</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1398,10 +1392,10 @@
         <v>46</v>
       </c>
       <c r="C45">
-        <v>1750</v>
+        <v>2649</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1412,10 +1406,10 @@
         <v>47</v>
       </c>
       <c r="C46">
-        <v>1925</v>
+        <v>4500</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1426,10 +1420,10 @@
         <v>48</v>
       </c>
       <c r="C47">
-        <v>2395</v>
+        <v>1900</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1440,10 +1434,10 @@
         <v>49</v>
       </c>
       <c r="C48">
-        <v>2400</v>
+        <v>1750</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1454,10 +1448,10 @@
         <v>50</v>
       </c>
       <c r="C49">
-        <v>3100</v>
+        <v>1925</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1468,10 +1462,10 @@
         <v>51</v>
       </c>
       <c r="C50">
-        <v>2000</v>
+        <v>3100</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1482,10 +1476,10 @@
         <v>52</v>
       </c>
       <c r="C51">
-        <v>2700</v>
+        <v>2000</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1496,10 +1490,10 @@
         <v>53</v>
       </c>
       <c r="C52">
-        <v>1895</v>
+        <v>2700</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1510,10 +1504,10 @@
         <v>54</v>
       </c>
       <c r="C53">
-        <v>1495</v>
+        <v>1895</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1524,10 +1518,10 @@
         <v>55</v>
       </c>
       <c r="C54">
-        <v>3995</v>
+        <v>1495</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1538,10 +1532,10 @@
         <v>56</v>
       </c>
       <c r="C55">
-        <v>2830</v>
+        <v>3995</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1552,10 +1546,10 @@
         <v>57</v>
       </c>
       <c r="C56">
-        <v>1275</v>
+        <v>2830</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1566,10 +1560,10 @@
         <v>58</v>
       </c>
       <c r="C57">
-        <v>2220</v>
+        <v>1275</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1583,7 +1577,7 @@
         <v>1400</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1597,7 +1591,7 @@
         <v>1325</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1611,7 +1605,7 @@
         <v>2200</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1625,7 +1619,7 @@
         <v>3560</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1639,7 +1633,7 @@
         <v>2830</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1653,21 +1647,7 @@
         <v>1750</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="1">
-        <v>22</v>
-      </c>
-      <c r="B64" t="s">
-        <v>65</v>
-      </c>
-      <c r="C64">
-        <v>2450</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1714,6 @@
     <hyperlink ref="D61" r:id="rId60"/>
     <hyperlink ref="D62" r:id="rId61"/>
     <hyperlink ref="D63" r:id="rId62"/>
-    <hyperlink ref="D64" r:id="rId63"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>